<commit_message>
Sun Jan  5 07:19:03 PM EST 2025 more ozone vtzp
</commit_message>
<xml_diff>
--- a/ozone/MAE_stacked_VTZP.xlsx
+++ b/ozone/MAE_stacked_VTZP.xlsx
@@ -452,10 +452,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.2851076882107093</v>
+        <v>0.1265419962205994</v>
       </c>
       <c r="C2" t="n">
-        <v>2.671180954222684</v>
+        <v>1.060363345747843</v>
       </c>
     </row>
     <row r="3">
@@ -465,10 +465,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2991427698894775</v>
+        <v>0.1732173909614563</v>
       </c>
       <c r="C3" t="n">
-        <v>3.086674271150811</v>
+        <v>3.108932044736805</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wed Jan 15 04:58:05 PM EST 2025 best ozone vtzp
</commit_message>
<xml_diff>
--- a/ozone/MAE_stacked_VTZP.xlsx
+++ b/ozone/MAE_stacked_VTZP.xlsx
@@ -452,10 +452,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.1265419962205994</v>
+        <v>0.1115939503977046</v>
       </c>
       <c r="C2" t="n">
-        <v>1.060363345747843</v>
+        <v>0.8631666532838131</v>
       </c>
     </row>
     <row r="3">
@@ -465,10 +465,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1732173909614563</v>
+        <v>0.1226217426068196</v>
       </c>
       <c r="C3" t="n">
-        <v>3.108932044736805</v>
+        <v>0.9714525084005331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>